<commit_message>
Pie chart with limited number of sales works and the bar chart works only for hard coded data.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eborye\Documents\SebliJAVA\HighChartsDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GBTC441018ur\IdeaProjects\HighChartsDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -707,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="1">
-        <v>12000</v>
+        <v>34200</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>17</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -727,7 +727,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="1">
-        <v>15000</v>
+        <v>38800</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>17</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="1">
-        <v>20000</v>
+        <v>43400</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>17</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -767,7 +767,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="1">
-        <v>25000</v>
+        <v>48000</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>17</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>10</v>
@@ -787,7 +787,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="8">
-        <v>30000</v>
+        <v>52600</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>17</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
@@ -807,7 +807,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="1">
-        <v>12000</v>
+        <v>57200</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>18</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -827,7 +827,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="1">
-        <v>15000</v>
+        <v>61800</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>18</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>
@@ -847,7 +847,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="1">
-        <v>20000</v>
+        <v>66400</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>18</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -867,7 +867,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="1">
-        <v>25000</v>
+        <v>71000</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>18</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>10</v>
@@ -887,7 +887,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="8">
-        <v>30000</v>
+        <v>75600</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>18</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -907,7 +907,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="1">
-        <v>12000</v>
+        <v>80200</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>19</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
@@ -927,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="1">
-        <v>15000</v>
+        <v>84800</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>19</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -947,7 +947,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="1">
-        <v>20000</v>
+        <v>89400</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>19</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -967,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="1">
-        <v>25000</v>
+        <v>94000</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>19</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>10</v>
@@ -987,7 +987,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="8">
-        <v>30000</v>
+        <v>98600</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>19</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -1007,7 +1007,7 @@
         <v>10</v>
       </c>
       <c r="E22" s="1">
-        <v>12000</v>
+        <v>103200</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>20</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
@@ -1027,7 +1027,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="1">
-        <v>15000</v>
+        <v>107800</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>20</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1047,7 +1047,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="1">
-        <v>20000</v>
+        <v>112400</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>20</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -1067,7 +1067,7 @@
         <v>14</v>
       </c>
       <c r="E25" s="1">
-        <v>25000</v>
+        <v>117000</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>20</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>10</v>
@@ -1087,7 +1087,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="8">
-        <v>30000</v>
+        <v>121600</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>20</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -1107,7 +1107,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="1">
-        <v>12000</v>
+        <v>126200</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>21</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
@@ -1127,7 +1127,7 @@
         <v>15</v>
       </c>
       <c r="E28" s="1">
-        <v>15000</v>
+        <v>130800</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>21</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
@@ -1147,7 +1147,7 @@
         <v>12</v>
       </c>
       <c r="E29" s="1">
-        <v>20000</v>
+        <v>135400</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>21</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>
@@ -1167,7 +1167,7 @@
         <v>14</v>
       </c>
       <c r="E30" s="1">
-        <v>25000</v>
+        <v>140000</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>21</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>10</v>
@@ -1187,7 +1187,7 @@
         <v>20</v>
       </c>
       <c r="E31" s="8">
-        <v>30000</v>
+        <v>144600</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>21</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
@@ -1207,7 +1207,7 @@
         <v>10</v>
       </c>
       <c r="E32" s="1">
-        <v>12000</v>
+        <v>149200</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>22</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
@@ -1227,7 +1227,7 @@
         <v>15</v>
       </c>
       <c r="E33" s="1">
-        <v>15000</v>
+        <v>153800</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>22</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>8</v>
@@ -1247,7 +1247,7 @@
         <v>12</v>
       </c>
       <c r="E34" s="1">
-        <v>20000</v>
+        <v>158400</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>22</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
@@ -1267,7 +1267,7 @@
         <v>14</v>
       </c>
       <c r="E35" s="1">
-        <v>25000</v>
+        <v>163000</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>10</v>
@@ -1287,7 +1287,7 @@
         <v>20</v>
       </c>
       <c r="E36" s="8">
-        <v>30000</v>
+        <v>167600</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>22</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>6</v>
@@ -1307,7 +1307,7 @@
         <v>10</v>
       </c>
       <c r="E37" s="1">
-        <v>12000</v>
+        <v>172200</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>23</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
@@ -1327,7 +1327,7 @@
         <v>15</v>
       </c>
       <c r="E38" s="1">
-        <v>15000</v>
+        <v>176800</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>23</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>8</v>
@@ -1347,7 +1347,7 @@
         <v>12</v>
       </c>
       <c r="E39" s="1">
-        <v>20000</v>
+        <v>181400</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>23</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>9</v>
@@ -1367,7 +1367,7 @@
         <v>14</v>
       </c>
       <c r="E40" s="1">
-        <v>25000</v>
+        <v>186000</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>23</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>10</v>
@@ -1387,7 +1387,7 @@
         <v>20</v>
       </c>
       <c r="E41" s="8">
-        <v>30000</v>
+        <v>190600</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>23</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>6</v>
@@ -1407,7 +1407,7 @@
         <v>10</v>
       </c>
       <c r="E42" s="1">
-        <v>12000</v>
+        <v>195200</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>24</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
@@ -1427,7 +1427,7 @@
         <v>15</v>
       </c>
       <c r="E43" s="1">
-        <v>15000</v>
+        <v>199800</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>24</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>8</v>
@@ -1447,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="E44" s="1">
-        <v>20000</v>
+        <v>204400</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>24</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>9</v>
@@ -1467,7 +1467,7 @@
         <v>14</v>
       </c>
       <c r="E45" s="1">
-        <v>25000</v>
+        <v>209000</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>24</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>10</v>
@@ -1487,7 +1487,7 @@
         <v>20</v>
       </c>
       <c r="E46" s="8">
-        <v>30000</v>
+        <v>213600</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>24</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>6</v>
@@ -1507,7 +1507,7 @@
         <v>10</v>
       </c>
       <c r="E47" s="1">
-        <v>12000</v>
+        <v>218200</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>25</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
@@ -1527,7 +1527,7 @@
         <v>15</v>
       </c>
       <c r="E48" s="1">
-        <v>15000</v>
+        <v>222800</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>25</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>8</v>
@@ -1547,7 +1547,7 @@
         <v>12</v>
       </c>
       <c r="E49" s="1">
-        <v>20000</v>
+        <v>227400</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>25</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>9</v>
@@ -1567,7 +1567,7 @@
         <v>14</v>
       </c>
       <c r="E50" s="1">
-        <v>25000</v>
+        <v>232000</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>25</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>10</v>
@@ -1587,7 +1587,7 @@
         <v>20</v>
       </c>
       <c r="E51" s="8">
-        <v>30000</v>
+        <v>236600</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>25</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>6</v>
@@ -1607,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="E52" s="1">
-        <v>12000</v>
+        <v>241200</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>26</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>7</v>
@@ -1627,7 +1627,7 @@
         <v>15</v>
       </c>
       <c r="E53" s="1">
-        <v>15000</v>
+        <v>245800</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>26</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>8</v>
@@ -1647,7 +1647,7 @@
         <v>12</v>
       </c>
       <c r="E54" s="1">
-        <v>20000</v>
+        <v>250400</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>26</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>9</v>
@@ -1667,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="E55" s="1">
-        <v>25000</v>
+        <v>255000</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>26</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>10</v>
@@ -1687,7 +1687,7 @@
         <v>20</v>
       </c>
       <c r="E56" s="8">
-        <v>30000</v>
+        <v>259600</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>26</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>6</v>
@@ -1707,7 +1707,7 @@
         <v>10</v>
       </c>
       <c r="E57" s="1">
-        <v>12000</v>
+        <v>264200</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>27</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>7</v>
@@ -1727,7 +1727,7 @@
         <v>15</v>
       </c>
       <c r="E58" s="1">
-        <v>15000</v>
+        <v>268800</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>27</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>8</v>
@@ -1747,7 +1747,7 @@
         <v>12</v>
       </c>
       <c r="E59" s="1">
-        <v>20000</v>
+        <v>273400</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>27</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>9</v>
@@ -1767,7 +1767,7 @@
         <v>14</v>
       </c>
       <c r="E60" s="1">
-        <v>25000</v>
+        <v>278000</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>27</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>10</v>
@@ -1787,7 +1787,7 @@
         <v>20</v>
       </c>
       <c r="E61" s="8">
-        <v>30000</v>
+        <v>282600</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Pie chart is almost done now the bar chert is left
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>april</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Testietm</t>
   </si>
 </sst>
 </file>
@@ -234,7 +240,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -258,9 +264,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -557,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E61"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,19 +678,19 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>20</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>30000</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -697,20 +701,20 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1">
-        <v>10</v>
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="8">
+        <v>12</v>
       </c>
       <c r="E7" s="1">
-        <v>34200</v>
+        <v>35000</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -718,16 +722,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>38800</v>
+        <v>34200</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>17</v>
@@ -738,16 +742,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
-        <v>43400</v>
+        <v>38800</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>17</v>
@@ -758,79 +762,79 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1">
-        <v>48000</v>
+        <v>43400</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="8">
-        <v>20</v>
-      </c>
-      <c r="E11" s="8">
-        <v>52600</v>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1">
+        <v>48000</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1">
-        <v>57200</v>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7">
+        <v>52600</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1">
-        <v>15</v>
+      <c r="B13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="8">
+        <v>12</v>
       </c>
       <c r="E13" s="1">
-        <v>61800</v>
+        <v>35000</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -838,16 +842,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1">
-        <v>66400</v>
+        <v>57200</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>18</v>
@@ -858,36 +862,36 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E15" s="1">
-        <v>71000</v>
+        <v>61800</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="8">
-        <v>20</v>
-      </c>
-      <c r="E16" s="8">
-        <v>75600</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1">
+        <v>66400</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>18</v>
@@ -898,39 +902,39 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1">
-        <v>80200</v>
+        <v>71000</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1">
-        <v>84800</v>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="7">
+        <v>20</v>
+      </c>
+      <c r="E18" s="7">
+        <v>75600</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,16 +942,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D19" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1">
-        <v>89400</v>
+        <v>80200</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>19</v>
@@ -958,36 +962,36 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D20" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="1">
-        <v>94000</v>
+        <v>84800</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="8">
-        <v>20</v>
-      </c>
-      <c r="E21" s="8">
-        <v>98600</v>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1">
+        <v>89400</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>19</v>
@@ -998,39 +1002,39 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E22" s="1">
-        <v>103200</v>
+        <v>94000</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="1">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1">
-        <v>107800</v>
+      <c r="B23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="7">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7">
+        <v>98600</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,16 +1042,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1">
-        <v>112400</v>
+        <v>103200</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>20</v>
@@ -1058,36 +1062,36 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D25" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E25" s="1">
-        <v>117000</v>
+        <v>107800</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="8">
-        <v>20</v>
-      </c>
-      <c r="E26" s="8">
-        <v>121600</v>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="1">
+        <v>12</v>
+      </c>
+      <c r="E26" s="1">
+        <v>112400</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>20</v>
@@ -1098,39 +1102,39 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D27" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E27" s="1">
-        <v>126200</v>
+        <v>117000</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="1">
-        <v>15</v>
-      </c>
-      <c r="E28" s="1">
-        <v>130800</v>
+      <c r="B28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="7">
+        <v>20</v>
+      </c>
+      <c r="E28" s="7">
+        <v>121600</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1138,16 +1142,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E29" s="1">
-        <v>135400</v>
+        <v>126200</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>21</v>
@@ -1158,36 +1162,36 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D30" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1">
-        <v>140000</v>
+        <v>130800</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="8">
-        <v>20</v>
-      </c>
-      <c r="E31" s="8">
-        <v>144600</v>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="1">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1">
+        <v>135400</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>21</v>
@@ -1198,39 +1202,39 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D32" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1">
-        <v>149200</v>
+        <v>140000</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="1">
-        <v>15</v>
-      </c>
-      <c r="E33" s="1">
-        <v>153800</v>
+      <c r="B33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="7">
+        <v>20</v>
+      </c>
+      <c r="E33" s="7">
+        <v>144600</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1238,16 +1242,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D34" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1">
-        <v>158400</v>
+        <v>149200</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>22</v>
@@ -1258,36 +1262,36 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D35" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E35" s="1">
-        <v>163000</v>
+        <v>153800</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="8">
-        <v>20</v>
-      </c>
-      <c r="E36" s="8">
-        <v>167600</v>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="1">
+        <v>12</v>
+      </c>
+      <c r="E36" s="1">
+        <v>158400</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>22</v>
@@ -1298,39 +1302,39 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E37" s="1">
-        <v>172200</v>
+        <v>163000</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="1">
-        <v>15</v>
-      </c>
-      <c r="E38" s="1">
-        <v>176800</v>
+      <c r="B38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="7">
+        <v>20</v>
+      </c>
+      <c r="E38" s="7">
+        <v>167600</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1338,16 +1342,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D39" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1">
-        <v>181400</v>
+        <v>172200</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>23</v>
@@ -1358,36 +1362,36 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D40" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E40" s="1">
-        <v>186000</v>
+        <v>176800</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="8">
-        <v>20</v>
-      </c>
-      <c r="E41" s="8">
-        <v>190600</v>
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="1">
+        <v>12</v>
+      </c>
+      <c r="E41" s="1">
+        <v>181400</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>23</v>
@@ -1398,39 +1402,39 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D42" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E42" s="1">
-        <v>195200</v>
+        <v>186000</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="1">
-        <v>15</v>
-      </c>
-      <c r="E43" s="1">
-        <v>199800</v>
+      <c r="B43" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="7">
+        <v>20</v>
+      </c>
+      <c r="E43" s="7">
+        <v>190600</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1438,16 +1442,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D44" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E44" s="1">
-        <v>204400</v>
+        <v>195200</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>24</v>
@@ -1458,36 +1462,36 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D45" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E45" s="1">
-        <v>209000</v>
+        <v>199800</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="8">
-        <v>20</v>
-      </c>
-      <c r="E46" s="8">
-        <v>213600</v>
+      <c r="B46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="1">
+        <v>12</v>
+      </c>
+      <c r="E46" s="1">
+        <v>204400</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>24</v>
@@ -1498,39 +1502,39 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D47" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E47" s="1">
-        <v>218200</v>
+        <v>209000</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="1">
-        <v>15</v>
-      </c>
-      <c r="E48" s="1">
-        <v>222800</v>
+      <c r="B48" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="7">
+        <v>20</v>
+      </c>
+      <c r="E48" s="7">
+        <v>213600</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1538,16 +1542,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D49" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E49" s="1">
-        <v>227400</v>
+        <v>218200</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>25</v>
@@ -1558,36 +1562,36 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D50" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E50" s="1">
-        <v>232000</v>
+        <v>222800</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="8">
-        <v>20</v>
-      </c>
-      <c r="E51" s="8">
-        <v>236600</v>
+      <c r="B51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="1">
+        <v>12</v>
+      </c>
+      <c r="E51" s="1">
+        <v>227400</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>25</v>
@@ -1598,39 +1602,39 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D52" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E52" s="1">
-        <v>241200</v>
+        <v>232000</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="1">
-        <v>15</v>
-      </c>
-      <c r="E53" s="1">
-        <v>245800</v>
+      <c r="B53" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="7">
+        <v>20</v>
+      </c>
+      <c r="E53" s="7">
+        <v>236600</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1638,16 +1642,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D54" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E54" s="1">
-        <v>250400</v>
+        <v>241200</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>26</v>
@@ -1658,36 +1662,36 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D55" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E55" s="1">
-        <v>255000</v>
+        <v>245800</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="8">
-        <v>20</v>
-      </c>
-      <c r="E56" s="8">
-        <v>259600</v>
+      <c r="B56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="1">
+        <v>12</v>
+      </c>
+      <c r="E56" s="1">
+        <v>250400</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>26</v>
@@ -1698,39 +1702,39 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D57" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E57" s="1">
-        <v>264200</v>
+        <v>255000</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="1">
-        <v>15</v>
-      </c>
-      <c r="E58" s="1">
-        <v>268800</v>
+      <c r="B58" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="7">
+        <v>20</v>
+      </c>
+      <c r="E58" s="7">
+        <v>259600</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1738,16 +1742,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D59" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E59" s="1">
-        <v>273400</v>
+        <v>264200</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>27</v>
@@ -1758,38 +1762,78 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D60" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E60" s="1">
-        <v>278000</v>
+        <v>268800</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="7">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="B61" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" s="8" t="s">
+      <c r="B61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" s="1">
+        <v>12</v>
+      </c>
+      <c r="E61" s="1">
+        <v>273400</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="1">
+        <v>14</v>
+      </c>
+      <c r="E62" s="1">
+        <v>278000</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D63" s="7">
         <v>20</v>
       </c>
-      <c r="E61" s="8">
+      <c r="E63" s="7">
         <v>282600</v>
       </c>
-      <c r="F61" s="6" t="s">
+      <c r="F63" s="6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The chart is done the label for the bar cahrt is left.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GBTC441018ur\IdeaProjects\HighChartsDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eborye\Documents\SebliJAVA\HighChartsDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -564,7 +564,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="E58" sqref="E58:E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +711,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="1">
-        <v>35000</v>
+        <v>12000</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>16</v>
@@ -731,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>34200</v>
+        <v>15000</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>17</v>
@@ -751,7 +751,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="1">
-        <v>38800</v>
+        <v>20000</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>17</v>
@@ -771,13 +771,13 @@
         <v>12</v>
       </c>
       <c r="E10" s="1">
-        <v>43400</v>
+        <v>25000</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -790,8 +790,8 @@
       <c r="D11" s="1">
         <v>14</v>
       </c>
-      <c r="E11" s="1">
-        <v>48000</v>
+      <c r="E11" s="7">
+        <v>30000</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>17</v>
@@ -811,7 +811,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="7">
-        <v>52600</v>
+        <v>40000</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>17</v>
@@ -831,7 +831,7 @@
         <v>12</v>
       </c>
       <c r="E13" s="1">
-        <v>35000</v>
+        <v>22000</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>17</v>
@@ -851,7 +851,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="1">
-        <v>57200</v>
+        <v>26000</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>18</v>
@@ -871,7 +871,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="1">
-        <v>61800</v>
+        <v>18000</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>18</v>
@@ -891,7 +891,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="1">
-        <v>66400</v>
+        <v>17000</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>18</v>
@@ -911,7 +911,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="1">
-        <v>71000</v>
+        <v>23000</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>18</v>
@@ -931,7 +931,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="7">
-        <v>75600</v>
+        <v>14000</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>18</v>
@@ -951,7 +951,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="1">
-        <v>80200</v>
+        <v>22000</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>19</v>
@@ -971,7 +971,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="1">
-        <v>84800</v>
+        <v>26000</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>19</v>
@@ -991,7 +991,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="1">
-        <v>89400</v>
+        <v>18000</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>19</v>
@@ -1011,7 +1011,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="1">
-        <v>94000</v>
+        <v>17000</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>19</v>
@@ -1030,14 +1030,14 @@
       <c r="D23" s="7">
         <v>20</v>
       </c>
-      <c r="E23" s="7">
-        <v>98600</v>
+      <c r="E23" s="1">
+        <v>23000</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1050,8 +1050,8 @@
       <c r="D24" s="1">
         <v>10</v>
       </c>
-      <c r="E24" s="1">
-        <v>103200</v>
+      <c r="E24" s="7">
+        <v>14000</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>20</v>
@@ -1071,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="1">
-        <v>107800</v>
+        <v>22000</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>20</v>
@@ -1091,7 +1091,7 @@
         <v>12</v>
       </c>
       <c r="E26" s="1">
-        <v>112400</v>
+        <v>26000</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>20</v>
@@ -1111,7 +1111,7 @@
         <v>14</v>
       </c>
       <c r="E27" s="1">
-        <v>117000</v>
+        <v>18000</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>20</v>
@@ -1130,8 +1130,8 @@
       <c r="D28" s="7">
         <v>20</v>
       </c>
-      <c r="E28" s="7">
-        <v>121600</v>
+      <c r="E28" s="1">
+        <v>17000</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>20</v>
@@ -1151,13 +1151,13 @@
         <v>10</v>
       </c>
       <c r="E29" s="1">
-        <v>126200</v>
+        <v>23000</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1170,8 +1170,8 @@
       <c r="D30" s="1">
         <v>15</v>
       </c>
-      <c r="E30" s="1">
-        <v>130800</v>
+      <c r="E30" s="7">
+        <v>14000</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>21</v>
@@ -1191,7 +1191,7 @@
         <v>12</v>
       </c>
       <c r="E31" s="1">
-        <v>135400</v>
+        <v>22000</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>21</v>
@@ -1211,7 +1211,7 @@
         <v>14</v>
       </c>
       <c r="E32" s="1">
-        <v>140000</v>
+        <v>26000</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>21</v>
@@ -1230,8 +1230,8 @@
       <c r="D33" s="7">
         <v>20</v>
       </c>
-      <c r="E33" s="7">
-        <v>144600</v>
+      <c r="E33" s="1">
+        <v>18000</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>21</v>
@@ -1251,7 +1251,7 @@
         <v>10</v>
       </c>
       <c r="E34" s="1">
-        <v>149200</v>
+        <v>17000</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>22</v>
@@ -1271,13 +1271,13 @@
         <v>15</v>
       </c>
       <c r="E35" s="1">
-        <v>153800</v>
+        <v>23000</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1290,8 +1290,8 @@
       <c r="D36" s="1">
         <v>12</v>
       </c>
-      <c r="E36" s="1">
-        <v>158400</v>
+      <c r="E36" s="7">
+        <v>14000</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>22</v>
@@ -1311,7 +1311,7 @@
         <v>14</v>
       </c>
       <c r="E37" s="1">
-        <v>163000</v>
+        <v>22000</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>22</v>
@@ -1330,8 +1330,8 @@
       <c r="D38" s="7">
         <v>20</v>
       </c>
-      <c r="E38" s="7">
-        <v>167600</v>
+      <c r="E38" s="1">
+        <v>26000</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>22</v>
@@ -1351,7 +1351,7 @@
         <v>10</v>
       </c>
       <c r="E39" s="1">
-        <v>172200</v>
+        <v>18000</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>23</v>
@@ -1371,7 +1371,7 @@
         <v>15</v>
       </c>
       <c r="E40" s="1">
-        <v>176800</v>
+        <v>17000</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>23</v>
@@ -1391,13 +1391,13 @@
         <v>12</v>
       </c>
       <c r="E41" s="1">
-        <v>181400</v>
+        <v>23000</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1410,8 +1410,8 @@
       <c r="D42" s="1">
         <v>14</v>
       </c>
-      <c r="E42" s="1">
-        <v>186000</v>
+      <c r="E42" s="7">
+        <v>14000</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>23</v>
@@ -1430,8 +1430,8 @@
       <c r="D43" s="7">
         <v>20</v>
       </c>
-      <c r="E43" s="7">
-        <v>190600</v>
+      <c r="E43" s="1">
+        <v>22000</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>23</v>
@@ -1451,7 +1451,7 @@
         <v>10</v>
       </c>
       <c r="E44" s="1">
-        <v>195200</v>
+        <v>26000</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>24</v>
@@ -1471,7 +1471,7 @@
         <v>15</v>
       </c>
       <c r="E45" s="1">
-        <v>199800</v>
+        <v>18000</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>24</v>
@@ -1491,7 +1491,7 @@
         <v>12</v>
       </c>
       <c r="E46" s="1">
-        <v>204400</v>
+        <v>17000</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>24</v>
@@ -1511,7 +1511,7 @@
         <v>14</v>
       </c>
       <c r="E47" s="1">
-        <v>209000</v>
+        <v>23000</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>24</v>
@@ -1531,7 +1531,7 @@
         <v>20</v>
       </c>
       <c r="E48" s="7">
-        <v>213600</v>
+        <v>14000</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>24</v>
@@ -1551,7 +1551,7 @@
         <v>10</v>
       </c>
       <c r="E49" s="1">
-        <v>218200</v>
+        <v>22000</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>25</v>
@@ -1571,7 +1571,7 @@
         <v>15</v>
       </c>
       <c r="E50" s="1">
-        <v>222800</v>
+        <v>26000</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>25</v>
@@ -1591,7 +1591,7 @@
         <v>12</v>
       </c>
       <c r="E51" s="1">
-        <v>227400</v>
+        <v>18000</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>25</v>
@@ -1611,7 +1611,7 @@
         <v>14</v>
       </c>
       <c r="E52" s="1">
-        <v>232000</v>
+        <v>17000</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>25</v>
@@ -1630,14 +1630,14 @@
       <c r="D53" s="7">
         <v>20</v>
       </c>
-      <c r="E53" s="7">
-        <v>236600</v>
+      <c r="E53" s="1">
+        <v>23000</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -1650,8 +1650,8 @@
       <c r="D54" s="1">
         <v>10</v>
       </c>
-      <c r="E54" s="1">
-        <v>241200</v>
+      <c r="E54" s="7">
+        <v>14000</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>26</v>
@@ -1671,7 +1671,7 @@
         <v>15</v>
       </c>
       <c r="E55" s="1">
-        <v>245800</v>
+        <v>22000</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>26</v>
@@ -1691,7 +1691,7 @@
         <v>12</v>
       </c>
       <c r="E56" s="1">
-        <v>250400</v>
+        <v>26000</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>26</v>
@@ -1711,7 +1711,7 @@
         <v>14</v>
       </c>
       <c r="E57" s="1">
-        <v>255000</v>
+        <v>18000</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>26</v>
@@ -1730,8 +1730,8 @@
       <c r="D58" s="7">
         <v>20</v>
       </c>
-      <c r="E58" s="7">
-        <v>259600</v>
+      <c r="E58" s="1">
+        <v>17000</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>26</v>
@@ -1751,13 +1751,13 @@
         <v>10</v>
       </c>
       <c r="E59" s="1">
-        <v>264200</v>
+        <v>23000</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -1770,8 +1770,8 @@
       <c r="D60" s="1">
         <v>15</v>
       </c>
-      <c r="E60" s="1">
-        <v>268800</v>
+      <c r="E60" s="7">
+        <v>14000</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>27</v>
@@ -1791,7 +1791,7 @@
         <v>12</v>
       </c>
       <c r="E61" s="1">
-        <v>273400</v>
+        <v>15000</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>27</v>
@@ -1811,7 +1811,7 @@
         <v>14</v>
       </c>
       <c r="E62" s="1">
-        <v>278000</v>
+        <v>13500</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>27</v>
@@ -1831,7 +1831,7 @@
         <v>20</v>
       </c>
       <c r="E63" s="7">
-        <v>282600</v>
+        <v>12000</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>27</v>

</xml_diff>